<commit_message>
some changes in chartflow
</commit_message>
<xml_diff>
--- a/Images/Conversation Chart Flow.xlsx
+++ b/Images/Conversation Chart Flow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\ai_chatbot\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C05F13-3C1E-4952-985E-33D16D9609FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59A23E-76A6-4829-89B5-CC63C36C455B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C508BC11-13A6-481C-8C9D-92C2A7B204D8}"/>
   </bookViews>
@@ -1066,10 +1066,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>482600</xdr:rowOff>
+      <xdr:rowOff>495300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -1092,8 +1092,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12547600" y="2247900"/>
-          <a:ext cx="1587500" cy="31750"/>
+          <a:off x="13030200" y="2260600"/>
+          <a:ext cx="1549400" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1301,8 +1301,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6540500" y="7416800"/>
-          <a:ext cx="25400" cy="635000"/>
+          <a:off x="6718300" y="7594600"/>
+          <a:ext cx="25400" cy="1168400"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2448,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6BDDDA-C780-4646-B0AF-3939A885ED1A}">
   <dimension ref="B3:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2569,15 +2569,15 @@
     </row>
     <row r="22" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:18" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J23" s="8" t="s">
@@ -2597,19 +2597,19 @@
         <v>18</v>
       </c>
       <c r="G26" s="4"/>
+      <c r="H26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="H27" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="I27" s="5"/>
-      <c r="J27" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="K27" s="5"/>
-      <c r="L27" s="5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="29" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="2:18" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>